<commit_message>
notes model, savenote, lodash
</commit_message>
<xml_diff>
--- a/backend/errors.xlsx
+++ b/backend/errors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\letsnote\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gauravjot\Projects\letsnote\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD2DFB5-FC36-4986-A438-94204185AB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B0C179-FA20-454B-987A-D7FB17DC4C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23547" yWindow="2511" windowWidth="22119" windowHeight="11693" xr2:uid="{1C311A9E-131F-4BA8-BC98-6422A11B8691}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{1C311A9E-131F-4BA8-BC98-6422A11B8691}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Code</t>
   </si>
@@ -105,6 +105,36 @@
   </si>
   <si>
     <t>Email verification token already consumed.</t>
+  </si>
+  <si>
+    <t>This note does not exist.</t>
+  </si>
+  <si>
+    <t>N0404</t>
+  </si>
+  <si>
+    <t>The user does not have or own that note.</t>
+  </si>
+  <si>
+    <t>backend.notes.views.readNote</t>
+  </si>
+  <si>
+    <t>N0407</t>
+  </si>
+  <si>
+    <t>backend.notes.views.deleteNote</t>
+  </si>
+  <si>
+    <t>User is trying to delete a note which does not exist or they do not own.</t>
+  </si>
+  <si>
+    <t>N0403</t>
+  </si>
+  <si>
+    <t>User is updating a note which does not exist.</t>
+  </si>
+  <si>
+    <t>backend.notes.views.updateNote</t>
   </si>
 </sst>
 </file>
@@ -486,20 +516,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F40D6E5-6094-4FA1-B79D-4B0314EDFB9B}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="33.59765625" customWidth="1"/>
-    <col min="3" max="3" width="46.8984375" customWidth="1"/>
+    <col min="3" max="3" width="46.86328125" customWidth="1"/>
     <col min="4" max="4" width="35.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -533,7 +563,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -550,7 +580,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -567,7 +597,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -584,7 +614,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -601,7 +631,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -618,158 +648,206 @@
         <v>401</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>